<commit_message>
added some financials and stock data, found useful package for auto downloading all stock data, next step work on own script to download financials
</commit_message>
<xml_diff>
--- a/SP500 stock list.xlsx
+++ b/SP500 stock list.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey\Desktop\Github\FinancialAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jleibowitz/Desktop/Github/FinancialAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="636" yWindow="1176" windowWidth="28164" windowHeight="16884" tabRatio="500"/>
+    <workbookView xWindow="660" yWindow="3320" windowWidth="19420" windowHeight="19600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$506</definedName>
+  </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -4428,7 +4431,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4457,12 +4460,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -4477,11 +4486,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4563,6 +4573,15 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t> (bull run) so naturally any random buying strategy will work and any random selling strategy will fail (key word being random). Perhaps include a go/no go decision based on the market performance (SandP) as a whole for the previous quarter to try and bring upthat #correct decrease.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>OR do it based on that specific sector performance (GICS sector or GICS subindustry performance)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -4841,24 +4860,24 @@
   <dimension ref="A1:K506"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.796875" customWidth="1"/>
-    <col min="3" max="3" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.19921875" customWidth="1"/>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
-    <col min="6" max="6" width="21.19921875" customWidth="1"/>
-    <col min="7" max="7" width="17.69921875" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
-    <col min="10" max="10" width="16.3984375" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1417</v>
       </c>
@@ -4890,8 +4909,8 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -4922,8 +4941,8 @@
         <v>0.23076923076923078</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
@@ -4956,8 +4975,8 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
@@ -4990,8 +5009,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
@@ -5024,8 +5043,8 @@
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
@@ -5058,8 +5077,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
@@ -5084,8 +5103,8 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
@@ -5110,8 +5129,8 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B9" t="s">
@@ -5136,8 +5155,8 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B10" t="s">
@@ -5162,8 +5181,8 @@
         <v>1932</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B11" t="s">
@@ -5188,7 +5207,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -5214,7 +5233,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -5240,7 +5259,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -5266,7 +5285,7 @@
         <v>1955</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -5292,7 +5311,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -5318,7 +5337,7 @@
         <v>1940</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -5344,7 +5363,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -5370,7 +5389,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -5396,7 +5415,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -5422,7 +5441,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -5448,7 +5467,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -5474,7 +5493,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -5500,7 +5519,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -5524,7 +5543,7 @@
       </c>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -5550,7 +5569,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -5576,7 +5595,7 @@
         <v>1917</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>102</v>
       </c>
@@ -5602,7 +5621,7 @@
         <v>1931</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>106</v>
       </c>
@@ -5628,7 +5647,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -5654,7 +5673,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>111</v>
       </c>
@@ -5678,7 +5697,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>116</v>
       </c>
@@ -5704,7 +5723,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>119</v>
       </c>
@@ -5730,7 +5749,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>123</v>
       </c>
@@ -5754,7 +5773,7 @@
       </c>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>126</v>
       </c>
@@ -5778,7 +5797,7 @@
         <v>1906</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>129</v>
       </c>
@@ -5802,7 +5821,7 @@
       </c>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>133</v>
       </c>
@@ -5826,7 +5845,7 @@
       </c>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>135</v>
       </c>
@@ -5850,7 +5869,7 @@
       </c>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>139</v>
       </c>
@@ -5874,7 +5893,7 @@
       </c>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>143</v>
       </c>
@@ -5898,7 +5917,7 @@
       </c>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>146</v>
       </c>
@@ -5922,7 +5941,7 @@
       </c>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>150</v>
       </c>
@@ -5946,7 +5965,7 @@
       </c>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -5970,7 +5989,7 @@
       </c>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>157</v>
       </c>
@@ -5994,7 +6013,7 @@
       </c>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>161</v>
       </c>
@@ -6018,7 +6037,7 @@
       </c>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>166</v>
       </c>
@@ -6042,7 +6061,7 @@
       </c>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>169</v>
       </c>
@@ -6066,7 +6085,7 @@
       </c>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>173</v>
       </c>
@@ -6090,7 +6109,7 @@
       </c>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>176</v>
       </c>
@@ -6114,7 +6133,7 @@
       </c>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>179</v>
       </c>
@@ -6138,7 +6157,7 @@
       </c>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>183</v>
       </c>
@@ -6162,7 +6181,7 @@
       </c>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>186</v>
       </c>
@@ -6186,7 +6205,7 @@
       </c>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>189</v>
       </c>
@@ -6210,7 +6229,7 @@
       </c>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>193</v>
       </c>
@@ -6234,7 +6253,7 @@
       </c>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>197</v>
       </c>
@@ -6258,7 +6277,7 @@
       </c>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>200</v>
       </c>
@@ -6282,7 +6301,7 @@
       </c>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>204</v>
       </c>
@@ -6306,7 +6325,7 @@
       </c>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>208</v>
       </c>
@@ -6332,7 +6351,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>211</v>
       </c>
@@ -6356,7 +6375,7 @@
       </c>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>214</v>
       </c>
@@ -6380,7 +6399,7 @@
       </c>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>217</v>
       </c>
@@ -6404,7 +6423,7 @@
       </c>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>222</v>
       </c>
@@ -6428,7 +6447,7 @@
       </c>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>225</v>
       </c>
@@ -6452,7 +6471,7 @@
       </c>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>228</v>
       </c>
@@ -6476,7 +6495,7 @@
       </c>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>232</v>
       </c>
@@ -6500,7 +6519,7 @@
       </c>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>235</v>
       </c>
@@ -6524,7 +6543,7 @@
       </c>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>239</v>
       </c>
@@ -6548,7 +6567,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>242</v>
       </c>
@@ -6572,7 +6591,7 @@
       </c>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>246</v>
       </c>
@@ -6596,7 +6615,7 @@
       </c>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>250</v>
       </c>
@@ -6620,7 +6639,7 @@
       </c>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>252</v>
       </c>
@@ -6646,7 +6665,7 @@
         <v>1931</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>255</v>
       </c>
@@ -6670,7 +6689,7 @@
       </c>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>259</v>
       </c>
@@ -6696,7 +6715,7 @@
         <v>1897</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>262</v>
       </c>
@@ -6720,7 +6739,7 @@
       </c>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>266</v>
       </c>
@@ -6744,7 +6763,7 @@
       </c>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>270</v>
       </c>
@@ -6768,7 +6787,7 @@
       </c>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>273</v>
       </c>
@@ -6792,7 +6811,7 @@
       </c>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>275</v>
       </c>
@@ -6816,7 +6835,7 @@
       </c>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>278</v>
       </c>
@@ -6840,7 +6859,7 @@
         <v>1916</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>281</v>
       </c>
@@ -6864,7 +6883,7 @@
       </c>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>284</v>
       </c>
@@ -6888,7 +6907,7 @@
       </c>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>287</v>
       </c>
@@ -6912,7 +6931,7 @@
       </c>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>289</v>
       </c>
@@ -6936,7 +6955,7 @@
       </c>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>292</v>
       </c>
@@ -6960,7 +6979,7 @@
       </c>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>294</v>
       </c>
@@ -6984,7 +7003,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>296</v>
       </c>
@@ -7008,7 +7027,7 @@
       </c>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>298</v>
       </c>
@@ -7035,7 +7054,7 @@
       </c>
       <c r="I86" s="2"/>
     </row>
-    <row r="87" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>301</v>
       </c>
@@ -7059,7 +7078,7 @@
       </c>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>305</v>
       </c>
@@ -7083,7 +7102,7 @@
       </c>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>309</v>
       </c>
@@ -7107,7 +7126,7 @@
       </c>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>313</v>
       </c>
@@ -7131,7 +7150,7 @@
       </c>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>315</v>
       </c>
@@ -7155,7 +7174,7 @@
       </c>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>317</v>
       </c>
@@ -7179,7 +7198,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>321</v>
       </c>
@@ -7205,7 +7224,7 @@
         <v>1935</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>324</v>
       </c>
@@ -7229,7 +7248,7 @@
       </c>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>327</v>
       </c>
@@ -7253,7 +7272,7 @@
       </c>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>329</v>
       </c>
@@ -7277,7 +7296,7 @@
       </c>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>333</v>
       </c>
@@ -7301,7 +7320,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>337</v>
       </c>
@@ -7325,7 +7344,7 @@
       </c>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>340</v>
       </c>
@@ -7349,7 +7368,7 @@
       </c>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>344</v>
       </c>
@@ -7373,7 +7392,7 @@
       </c>
       <c r="H100" s="2"/>
     </row>
-    <row r="101" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>347</v>
       </c>
@@ -7397,7 +7416,7 @@
       </c>
       <c r="H101" s="2"/>
     </row>
-    <row r="102" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>350</v>
       </c>
@@ -7421,7 +7440,7 @@
       </c>
       <c r="H102" s="2"/>
     </row>
-    <row r="103" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>353</v>
       </c>
@@ -7445,7 +7464,7 @@
       </c>
       <c r="H103" s="2"/>
     </row>
-    <row r="104" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>355</v>
       </c>
@@ -7469,7 +7488,7 @@
       </c>
       <c r="H104" s="2"/>
     </row>
-    <row r="105" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>358</v>
       </c>
@@ -7493,7 +7512,7 @@
       </c>
       <c r="H105" s="2"/>
     </row>
-    <row r="106" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>362</v>
       </c>
@@ -7517,7 +7536,7 @@
       </c>
       <c r="H106" s="2"/>
     </row>
-    <row r="107" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>365</v>
       </c>
@@ -7541,7 +7560,7 @@
       </c>
       <c r="H107" s="2"/>
     </row>
-    <row r="108" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>369</v>
       </c>
@@ -7565,7 +7584,7 @@
       </c>
       <c r="H108" s="2"/>
     </row>
-    <row r="109" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>373</v>
       </c>
@@ -7589,7 +7608,7 @@
         <v>1879</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>377</v>
       </c>
@@ -7613,7 +7632,7 @@
       </c>
       <c r="H110" s="2"/>
     </row>
-    <row r="111" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>380</v>
       </c>
@@ -7637,7 +7656,7 @@
       </c>
       <c r="H111" s="2"/>
     </row>
-    <row r="112" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>383</v>
       </c>
@@ -7661,7 +7680,7 @@
       </c>
       <c r="H112" s="2"/>
     </row>
-    <row r="113" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>387</v>
       </c>
@@ -7685,7 +7704,7 @@
       </c>
       <c r="H113" s="2"/>
     </row>
-    <row r="114" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>390</v>
       </c>
@@ -7709,7 +7728,7 @@
       </c>
       <c r="H114" s="2"/>
     </row>
-    <row r="115" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>392</v>
       </c>
@@ -7733,7 +7752,7 @@
       </c>
       <c r="H115" s="2"/>
     </row>
-    <row r="116" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>395</v>
       </c>
@@ -7757,7 +7776,7 @@
       </c>
       <c r="H116" s="2"/>
     </row>
-    <row r="117" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>399</v>
       </c>
@@ -7781,7 +7800,7 @@
       </c>
       <c r="H117" s="2"/>
     </row>
-    <row r="118" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>402</v>
       </c>
@@ -7805,7 +7824,7 @@
       </c>
       <c r="H118" s="2"/>
     </row>
-    <row r="119" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>404</v>
       </c>
@@ -7829,7 +7848,7 @@
       </c>
       <c r="H119" s="2"/>
     </row>
-    <row r="120" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>407</v>
       </c>
@@ -7853,7 +7872,7 @@
       </c>
       <c r="H120" s="2"/>
     </row>
-    <row r="121" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>410</v>
       </c>
@@ -7879,7 +7898,7 @@
         <v>1913</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>413</v>
       </c>
@@ -7903,7 +7922,7 @@
       </c>
       <c r="H122" s="2"/>
     </row>
-    <row r="123" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>415</v>
       </c>
@@ -7927,7 +7946,7 @@
       </c>
       <c r="H123" s="2"/>
     </row>
-    <row r="124" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>418</v>
       </c>
@@ -7951,7 +7970,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>422</v>
       </c>
@@ -7975,7 +7994,7 @@
       </c>
       <c r="H125" s="2"/>
     </row>
-    <row r="126" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>425</v>
       </c>
@@ -7999,7 +8018,7 @@
         <v>1806</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>427</v>
       </c>
@@ -8023,7 +8042,7 @@
       </c>
       <c r="H127" s="2"/>
     </row>
-    <row r="128" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>430</v>
       </c>
@@ -8047,7 +8066,7 @@
       </c>
       <c r="H128" s="2"/>
     </row>
-    <row r="129" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>432</v>
       </c>
@@ -8071,7 +8090,7 @@
       </c>
       <c r="H129" s="2"/>
     </row>
-    <row r="130" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>434</v>
       </c>
@@ -8095,7 +8114,7 @@
       </c>
       <c r="H130" s="2"/>
     </row>
-    <row r="131" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>437</v>
       </c>
@@ -8119,7 +8138,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>439</v>
       </c>
@@ -8143,7 +8162,7 @@
         <v>1823</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>441</v>
       </c>
@@ -8167,7 +8186,7 @@
       </c>
       <c r="H133" s="2"/>
     </row>
-    <row r="134" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>444</v>
       </c>
@@ -8191,7 +8210,7 @@
       </c>
       <c r="H134" s="2"/>
     </row>
-    <row r="135" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>447</v>
       </c>
@@ -8215,7 +8234,7 @@
         <v>1851</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>450</v>
       </c>
@@ -8239,7 +8258,7 @@
       </c>
       <c r="H136" s="2"/>
     </row>
-    <row r="137" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>454</v>
       </c>
@@ -8263,7 +8282,7 @@
       </c>
       <c r="H137" s="2"/>
     </row>
-    <row r="138" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>457</v>
       </c>
@@ -8287,7 +8306,7 @@
       </c>
       <c r="H138" s="2"/>
     </row>
-    <row r="139" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>459</v>
       </c>
@@ -8313,7 +8332,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>463</v>
       </c>
@@ -8339,7 +8358,7 @@
         <v>1919</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>467</v>
       </c>
@@ -8363,7 +8382,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>471</v>
       </c>
@@ -8387,7 +8406,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>474</v>
       </c>
@@ -8411,7 +8430,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>477</v>
       </c>
@@ -8435,7 +8454,7 @@
         <v>1938</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>480</v>
       </c>
@@ -8459,7 +8478,7 @@
       </c>
       <c r="H145" s="2"/>
     </row>
-    <row r="146" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>483</v>
       </c>
@@ -8483,7 +8502,7 @@
         <v>1837</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>487</v>
       </c>
@@ -8507,7 +8526,7 @@
       </c>
       <c r="H147" s="2"/>
     </row>
-    <row r="148" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>489</v>
       </c>
@@ -8531,7 +8550,7 @@
       </c>
       <c r="H148" s="2"/>
     </row>
-    <row r="149" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>492</v>
       </c>
@@ -8555,7 +8574,7 @@
       </c>
       <c r="H149" s="2"/>
     </row>
-    <row r="150" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>495</v>
       </c>
@@ -8579,7 +8598,7 @@
       </c>
       <c r="H150" s="2"/>
     </row>
-    <row r="151" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>497</v>
       </c>
@@ -8603,7 +8622,7 @@
       </c>
       <c r="H151" s="2"/>
     </row>
-    <row r="152" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>500</v>
       </c>
@@ -8627,7 +8646,7 @@
       </c>
       <c r="H152" s="2"/>
     </row>
-    <row r="153" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>503</v>
       </c>
@@ -8651,7 +8670,7 @@
       </c>
       <c r="H153" s="2"/>
     </row>
-    <row r="154" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>505</v>
       </c>
@@ -8675,7 +8694,7 @@
       </c>
       <c r="H154" s="2"/>
     </row>
-    <row r="155" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>508</v>
       </c>
@@ -8699,7 +8718,7 @@
       </c>
       <c r="H155" s="2"/>
     </row>
-    <row r="156" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>512</v>
       </c>
@@ -8723,7 +8742,7 @@
       </c>
       <c r="H156" s="2"/>
     </row>
-    <row r="157" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>515</v>
       </c>
@@ -8747,7 +8766,7 @@
         <v>1983</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>517</v>
       </c>
@@ -8771,7 +8790,7 @@
       </c>
       <c r="H158" s="2"/>
     </row>
-    <row r="159" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>520</v>
       </c>
@@ -8795,7 +8814,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>524</v>
       </c>
@@ -8819,7 +8838,7 @@
       </c>
       <c r="H160" s="2"/>
     </row>
-    <row r="161" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>526</v>
       </c>
@@ -8843,7 +8862,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>529</v>
       </c>
@@ -8867,7 +8886,7 @@
       </c>
       <c r="H162" s="2"/>
     </row>
-    <row r="163" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>532</v>
       </c>
@@ -8891,7 +8910,7 @@
       </c>
       <c r="H163" s="2"/>
     </row>
-    <row r="164" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>534</v>
       </c>
@@ -8915,7 +8934,7 @@
       </c>
       <c r="H164" s="2"/>
     </row>
-    <row r="165" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>536</v>
       </c>
@@ -8939,7 +8958,7 @@
       </c>
       <c r="H165" s="2"/>
     </row>
-    <row r="166" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>538</v>
       </c>
@@ -8963,7 +8982,7 @@
       </c>
       <c r="H166" s="2"/>
     </row>
-    <row r="167" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>541</v>
       </c>
@@ -8987,7 +9006,7 @@
         <v>1911</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>543</v>
       </c>
@@ -9011,7 +9030,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>545</v>
       </c>
@@ -9035,7 +9054,7 @@
       </c>
       <c r="H169" s="2"/>
     </row>
-    <row r="170" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>547</v>
       </c>
@@ -9059,7 +9078,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>550</v>
       </c>
@@ -9083,7 +9102,7 @@
       </c>
       <c r="H171" s="2"/>
     </row>
-    <row r="172" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>553</v>
       </c>
@@ -9107,7 +9126,7 @@
       </c>
       <c r="H172" s="2"/>
     </row>
-    <row r="173" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>556</v>
       </c>
@@ -9133,7 +9152,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>559</v>
       </c>
@@ -9157,7 +9176,7 @@
         <v>1913</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>562</v>
       </c>
@@ -9181,7 +9200,7 @@
       </c>
       <c r="H175" s="2"/>
     </row>
-    <row r="176" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>566</v>
       </c>
@@ -9205,7 +9224,7 @@
       </c>
       <c r="H176" s="2"/>
     </row>
-    <row r="177" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>568</v>
       </c>
@@ -9229,7 +9248,7 @@
       </c>
       <c r="H177" s="2"/>
     </row>
-    <row r="178" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>571</v>
       </c>
@@ -9253,7 +9272,7 @@
       </c>
       <c r="H178" s="2"/>
     </row>
-    <row r="179" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>574</v>
       </c>
@@ -9277,7 +9296,7 @@
       </c>
       <c r="H179" s="2"/>
     </row>
-    <row r="180" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>576</v>
       </c>
@@ -9301,7 +9320,7 @@
       </c>
       <c r="H180" s="2"/>
     </row>
-    <row r="181" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>578</v>
       </c>
@@ -9325,7 +9344,7 @@
       </c>
       <c r="H181" s="2"/>
     </row>
-    <row r="182" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>581</v>
       </c>
@@ -9349,7 +9368,7 @@
       </c>
       <c r="H182" s="2"/>
     </row>
-    <row r="183" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>583</v>
       </c>
@@ -9375,7 +9394,7 @@
         <v>1909</v>
       </c>
     </row>
-    <row r="184" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>585</v>
       </c>
@@ -9399,7 +9418,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>588</v>
       </c>
@@ -9423,7 +9442,7 @@
       </c>
       <c r="H185" s="2"/>
     </row>
-    <row r="186" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>592</v>
       </c>
@@ -9447,7 +9466,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="187" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>594</v>
       </c>
@@ -9471,7 +9490,7 @@
       </c>
       <c r="H187" s="2"/>
     </row>
-    <row r="188" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>597</v>
       </c>
@@ -9495,7 +9514,7 @@
       </c>
       <c r="H188" s="2"/>
     </row>
-    <row r="189" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>599</v>
       </c>
@@ -9519,7 +9538,7 @@
       </c>
       <c r="H189" s="2"/>
     </row>
-    <row r="190" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>602</v>
       </c>
@@ -9543,7 +9562,7 @@
       </c>
       <c r="H190" s="2"/>
     </row>
-    <row r="191" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>605</v>
       </c>
@@ -9567,7 +9586,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="192" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>608</v>
       </c>
@@ -9594,7 +9613,7 @@
       </c>
       <c r="I192" s="2"/>
     </row>
-    <row r="193" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>610</v>
       </c>
@@ -9618,7 +9637,7 @@
       </c>
       <c r="H193" s="2"/>
     </row>
-    <row r="194" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>613</v>
       </c>
@@ -9642,7 +9661,7 @@
       </c>
       <c r="H194" s="2"/>
     </row>
-    <row r="195" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>616</v>
       </c>
@@ -9666,7 +9685,7 @@
       </c>
       <c r="H195" s="2"/>
     </row>
-    <row r="196" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>620</v>
       </c>
@@ -9690,7 +9709,7 @@
       </c>
       <c r="H196" s="2"/>
     </row>
-    <row r="197" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>622</v>
       </c>
@@ -9714,7 +9733,7 @@
       </c>
       <c r="H197" s="2"/>
     </row>
-    <row r="198" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>624</v>
       </c>
@@ -9738,7 +9757,7 @@
         <v>1858</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>627</v>
       </c>
@@ -9762,7 +9781,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="200" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>630</v>
       </c>
@@ -9786,7 +9805,7 @@
       </c>
       <c r="H200" s="2"/>
     </row>
-    <row r="201" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>633</v>
       </c>
@@ -9810,7 +9829,7 @@
       </c>
       <c r="H201" s="2"/>
     </row>
-    <row r="202" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>637</v>
       </c>
@@ -9834,7 +9853,7 @@
       </c>
       <c r="H202" s="2"/>
     </row>
-    <row r="203" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>639</v>
       </c>
@@ -9858,7 +9877,7 @@
       </c>
       <c r="H203" s="2"/>
     </row>
-    <row r="204" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>642</v>
       </c>
@@ -9882,7 +9901,7 @@
       </c>
       <c r="H204" s="2"/>
     </row>
-    <row r="205" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>644</v>
       </c>
@@ -9906,7 +9925,7 @@
       </c>
       <c r="H205" s="2"/>
     </row>
-    <row r="206" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>647</v>
       </c>
@@ -9930,7 +9949,7 @@
         <v>1903</v>
       </c>
     </row>
-    <row r="207" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>651</v>
       </c>
@@ -9954,7 +9973,7 @@
       </c>
       <c r="H207" s="2"/>
     </row>
-    <row r="208" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>654</v>
       </c>
@@ -9978,7 +9997,7 @@
       </c>
       <c r="H208" s="2"/>
     </row>
-    <row r="209" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>656</v>
       </c>
@@ -10002,7 +10021,7 @@
         <v>1947</v>
       </c>
     </row>
-    <row r="210" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>659</v>
       </c>
@@ -10026,7 +10045,7 @@
         <v>1912</v>
       </c>
     </row>
-    <row r="211" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>663</v>
       </c>
@@ -10050,7 +10069,7 @@
       </c>
       <c r="H211" s="2"/>
     </row>
-    <row r="212" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>665</v>
       </c>
@@ -10074,7 +10093,7 @@
       </c>
       <c r="H212" s="2"/>
     </row>
-    <row r="213" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>669</v>
       </c>
@@ -10098,7 +10117,7 @@
       </c>
       <c r="H213" s="2"/>
     </row>
-    <row r="214" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>671</v>
       </c>
@@ -10122,7 +10141,7 @@
         <v>1899</v>
       </c>
     </row>
-    <row r="215" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>674</v>
       </c>
@@ -10146,7 +10165,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="216" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>676</v>
       </c>
@@ -10170,7 +10189,7 @@
       </c>
       <c r="H216" s="2"/>
     </row>
-    <row r="217" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>678</v>
       </c>
@@ -10196,7 +10215,7 @@
         <v>1856</v>
       </c>
     </row>
-    <row r="218" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>681</v>
       </c>
@@ -10220,7 +10239,7 @@
       </c>
       <c r="H218" s="2"/>
     </row>
-    <row r="219" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>683</v>
       </c>
@@ -10246,7 +10265,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="220" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>685</v>
       </c>
@@ -10270,7 +10289,7 @@
       </c>
       <c r="H220" s="2"/>
     </row>
-    <row r="221" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>688</v>
       </c>
@@ -10294,7 +10313,7 @@
       </c>
       <c r="H221" s="2"/>
     </row>
-    <row r="222" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>690</v>
       </c>
@@ -10318,7 +10337,7 @@
       </c>
       <c r="H222" s="2"/>
     </row>
-    <row r="223" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>692</v>
       </c>
@@ -10342,7 +10361,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="224" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>695</v>
       </c>
@@ -10366,7 +10385,7 @@
       </c>
       <c r="H224" s="2"/>
     </row>
-    <row r="225" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>698</v>
       </c>
@@ -10390,7 +10409,7 @@
         <v>1919</v>
       </c>
     </row>
-    <row r="226" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>700</v>
       </c>
@@ -10414,7 +10433,7 @@
       </c>
       <c r="H226" s="2"/>
     </row>
-    <row r="227" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>703</v>
       </c>
@@ -10438,7 +10457,7 @@
         <v>1903</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>706</v>
       </c>
@@ -10462,7 +10481,7 @@
       </c>
       <c r="H228" s="2"/>
     </row>
-    <row r="229" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>709</v>
       </c>
@@ -10484,7 +10503,7 @@
       </c>
       <c r="H229" s="2"/>
     </row>
-    <row r="230" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>711</v>
       </c>
@@ -10508,7 +10527,7 @@
       </c>
       <c r="H230" s="2"/>
     </row>
-    <row r="231" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>715</v>
       </c>
@@ -10532,7 +10551,7 @@
       </c>
       <c r="H231" s="2"/>
     </row>
-    <row r="232" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>717</v>
       </c>
@@ -10556,7 +10575,7 @@
       </c>
       <c r="H232" s="2"/>
     </row>
-    <row r="233" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>721</v>
       </c>
@@ -10580,7 +10599,7 @@
       </c>
       <c r="H233" s="2"/>
     </row>
-    <row r="234" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>725</v>
       </c>
@@ -10604,7 +10623,7 @@
       </c>
       <c r="H234" s="2"/>
     </row>
-    <row r="235" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>728</v>
       </c>
@@ -10628,7 +10647,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>731</v>
       </c>
@@ -10652,7 +10671,7 @@
       </c>
       <c r="H236" s="2"/>
     </row>
-    <row r="237" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>733</v>
       </c>
@@ -10676,7 +10695,7 @@
       </c>
       <c r="H237" s="2"/>
     </row>
-    <row r="238" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>735</v>
       </c>
@@ -10700,7 +10719,7 @@
       </c>
       <c r="H238" s="2"/>
     </row>
-    <row r="239" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>737</v>
       </c>
@@ -10726,7 +10745,7 @@
         <v>1947</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>739</v>
       </c>
@@ -10750,7 +10769,7 @@
       </c>
       <c r="H240" s="2"/>
     </row>
-    <row r="241" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>742</v>
       </c>
@@ -10774,7 +10793,7 @@
       </c>
       <c r="H241" s="2"/>
     </row>
-    <row r="242" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>745</v>
       </c>
@@ -10800,7 +10819,7 @@
         <v>1906</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>748</v>
       </c>
@@ -10824,7 +10843,7 @@
       </c>
       <c r="H243" s="2"/>
     </row>
-    <row r="244" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>751</v>
       </c>
@@ -10848,7 +10867,7 @@
       </c>
       <c r="H244" s="2"/>
     </row>
-    <row r="245" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>755</v>
       </c>
@@ -10874,7 +10893,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>758</v>
       </c>
@@ -10898,7 +10917,7 @@
         <v>1961</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>760</v>
       </c>
@@ -10922,7 +10941,7 @@
         <v>1866</v>
       </c>
     </row>
-    <row r="248" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>762</v>
       </c>
@@ -10946,7 +10965,7 @@
       </c>
       <c r="H248" s="2"/>
     </row>
-    <row r="249" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>765</v>
       </c>
@@ -10970,7 +10989,7 @@
       </c>
       <c r="H249" s="2"/>
     </row>
-    <row r="250" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>768</v>
       </c>
@@ -10994,7 +11013,7 @@
       </c>
       <c r="H250" s="2"/>
     </row>
-    <row r="251" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>770</v>
       </c>
@@ -11018,7 +11037,7 @@
       </c>
       <c r="H251" s="2"/>
     </row>
-    <row r="252" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>773</v>
       </c>
@@ -11042,7 +11061,7 @@
       </c>
       <c r="H252" s="2"/>
     </row>
-    <row r="253" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>777</v>
       </c>
@@ -11066,7 +11085,7 @@
       </c>
       <c r="H253" s="2"/>
     </row>
-    <row r="254" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>779</v>
       </c>
@@ -11090,7 +11109,7 @@
       </c>
       <c r="H254" s="2"/>
     </row>
-    <row r="255" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>781</v>
       </c>
@@ -11114,7 +11133,7 @@
       </c>
       <c r="H255" s="2"/>
     </row>
-    <row r="256" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>783</v>
       </c>
@@ -11138,7 +11157,7 @@
         <v>1911</v>
       </c>
     </row>
-    <row r="257" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>786</v>
       </c>
@@ -11162,7 +11181,7 @@
       </c>
       <c r="H257" s="2"/>
     </row>
-    <row r="258" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>789</v>
       </c>
@@ -11186,7 +11205,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="259" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>791</v>
       </c>
@@ -11210,7 +11229,7 @@
       </c>
       <c r="H259" s="2"/>
     </row>
-    <row r="260" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>794</v>
       </c>
@@ -11234,7 +11253,7 @@
       </c>
       <c r="H260" s="2"/>
     </row>
-    <row r="261" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>796</v>
       </c>
@@ -11258,7 +11277,7 @@
       </c>
       <c r="H261" s="2"/>
     </row>
-    <row r="262" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>798</v>
       </c>
@@ -11282,7 +11301,7 @@
       </c>
       <c r="H262" s="2"/>
     </row>
-    <row r="263" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>800</v>
       </c>
@@ -11306,7 +11325,7 @@
       </c>
       <c r="H263" s="2"/>
     </row>
-    <row r="264" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>802</v>
       </c>
@@ -11330,7 +11349,7 @@
       </c>
       <c r="H264" s="2"/>
     </row>
-    <row r="265" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>806</v>
       </c>
@@ -11354,7 +11373,7 @@
       </c>
       <c r="H265" s="2"/>
     </row>
-    <row r="266" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>810</v>
       </c>
@@ -11378,7 +11397,7 @@
       </c>
       <c r="H266" s="2"/>
     </row>
-    <row r="267" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>812</v>
       </c>
@@ -11402,7 +11421,7 @@
       </c>
       <c r="H267" s="2"/>
     </row>
-    <row r="268" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>814</v>
       </c>
@@ -11426,7 +11445,7 @@
       </c>
       <c r="H268" s="2"/>
     </row>
-    <row r="269" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>818</v>
       </c>
@@ -11450,7 +11469,7 @@
       </c>
       <c r="H269" s="2"/>
     </row>
-    <row r="270" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>820</v>
       </c>
@@ -11474,7 +11493,7 @@
       </c>
       <c r="H270" s="2"/>
     </row>
-    <row r="271" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>823</v>
       </c>
@@ -11500,7 +11519,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="272" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>826</v>
       </c>
@@ -11524,7 +11543,7 @@
       </c>
       <c r="H272" s="2"/>
     </row>
-    <row r="273" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>829</v>
       </c>
@@ -11548,7 +11567,7 @@
       </c>
       <c r="H273" s="2"/>
     </row>
-    <row r="274" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>831</v>
       </c>
@@ -11572,7 +11591,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="275" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>833</v>
       </c>
@@ -11596,7 +11615,7 @@
       </c>
       <c r="H275" s="2"/>
     </row>
-    <row r="276" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>835</v>
       </c>
@@ -11620,7 +11639,7 @@
         <v>1906</v>
       </c>
     </row>
-    <row r="277" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>838</v>
       </c>
@@ -11644,7 +11663,7 @@
       </c>
       <c r="H277" s="2"/>
     </row>
-    <row r="278" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>841</v>
       </c>
@@ -11668,7 +11687,7 @@
         <v>1872</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>843</v>
       </c>
@@ -11692,7 +11711,7 @@
       </c>
       <c r="H279" s="2"/>
     </row>
-    <row r="280" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>846</v>
       </c>
@@ -11716,7 +11735,7 @@
       </c>
       <c r="H280" s="2"/>
     </row>
-    <row r="281" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>849</v>
       </c>
@@ -11740,7 +11759,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="282" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>853</v>
       </c>
@@ -11764,7 +11783,7 @@
         <v>1962</v>
       </c>
     </row>
-    <row r="283" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>856</v>
       </c>
@@ -11788,7 +11807,7 @@
       </c>
       <c r="H283" s="2"/>
     </row>
-    <row r="284" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>858</v>
       </c>
@@ -11812,7 +11831,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="285" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>861</v>
       </c>
@@ -11836,7 +11855,7 @@
       </c>
       <c r="H285" s="2"/>
     </row>
-    <row r="286" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>863</v>
       </c>
@@ -11860,7 +11879,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="287" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>865</v>
       </c>
@@ -11884,7 +11903,7 @@
       </c>
       <c r="H287" s="2"/>
     </row>
-    <row r="288" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>868</v>
       </c>
@@ -11908,7 +11927,7 @@
       </c>
       <c r="H288" s="2"/>
     </row>
-    <row r="289" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>871</v>
       </c>
@@ -11932,7 +11951,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="290" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>875</v>
       </c>
@@ -11956,7 +11975,7 @@
       </c>
       <c r="H290" s="2"/>
     </row>
-    <row r="291" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>877</v>
       </c>
@@ -11982,7 +12001,7 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="292" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>879</v>
       </c>
@@ -12006,7 +12025,7 @@
       </c>
       <c r="H292" s="2"/>
     </row>
-    <row r="293" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>882</v>
       </c>
@@ -12030,7 +12049,7 @@
       </c>
       <c r="H293" s="2"/>
     </row>
-    <row r="294" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>885</v>
       </c>
@@ -12054,7 +12073,7 @@
       </c>
       <c r="H294" s="2"/>
     </row>
-    <row r="295" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>887</v>
       </c>
@@ -12076,7 +12095,7 @@
       </c>
       <c r="H295" s="2"/>
     </row>
-    <row r="296" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>889</v>
       </c>
@@ -12102,7 +12121,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="297" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>893</v>
       </c>
@@ -12126,7 +12145,7 @@
       </c>
       <c r="H297" s="2"/>
     </row>
-    <row r="298" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>896</v>
       </c>
@@ -12150,7 +12169,7 @@
         <v>1856</v>
       </c>
     </row>
-    <row r="299" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>899</v>
       </c>
@@ -12174,7 +12193,7 @@
       </c>
       <c r="H299" s="2"/>
     </row>
-    <row r="300" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>901</v>
       </c>
@@ -12198,7 +12217,7 @@
         <v>1929</v>
       </c>
     </row>
-    <row r="301" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>904</v>
       </c>
@@ -12222,7 +12241,7 @@
       </c>
       <c r="H301" s="2"/>
     </row>
-    <row r="302" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>906</v>
       </c>
@@ -12246,7 +12265,7 @@
       </c>
       <c r="H302" s="2"/>
     </row>
-    <row r="303" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>909</v>
       </c>
@@ -12270,7 +12289,7 @@
         <v>1927</v>
       </c>
     </row>
-    <row r="304" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>911</v>
       </c>
@@ -12294,7 +12313,7 @@
       </c>
       <c r="H304" s="2"/>
     </row>
-    <row r="305" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>913</v>
       </c>
@@ -12318,7 +12337,7 @@
       </c>
       <c r="H305" s="2"/>
     </row>
-    <row r="306" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>917</v>
       </c>
@@ -12342,7 +12361,7 @@
       </c>
       <c r="H306" s="2"/>
     </row>
-    <row r="307" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>920</v>
       </c>
@@ -12366,7 +12385,7 @@
       </c>
       <c r="H307" s="2"/>
     </row>
-    <row r="308" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>923</v>
       </c>
@@ -12390,7 +12409,7 @@
       </c>
       <c r="H308" s="2"/>
     </row>
-    <row r="309" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>926</v>
       </c>
@@ -12414,7 +12433,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="310" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>929</v>
       </c>
@@ -12440,7 +12459,7 @@
         <v>1940</v>
       </c>
     </row>
-    <row r="311" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>932</v>
       </c>
@@ -12464,7 +12483,7 @@
         <v>1833</v>
       </c>
     </row>
-    <row r="312" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>934</v>
       </c>
@@ -12488,7 +12507,7 @@
       </c>
       <c r="H312" s="2"/>
     </row>
-    <row r="313" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>937</v>
       </c>
@@ -12512,7 +12531,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="314" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>940</v>
       </c>
@@ -12536,7 +12555,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="315" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>942</v>
       </c>
@@ -12560,7 +12579,7 @@
       </c>
       <c r="H315" s="2"/>
     </row>
-    <row r="316" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>944</v>
       </c>
@@ -12584,7 +12603,7 @@
       </c>
       <c r="H316" s="2"/>
     </row>
-    <row r="317" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>948</v>
       </c>
@@ -12608,7 +12627,7 @@
       </c>
       <c r="H317" s="2"/>
     </row>
-    <row r="318" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>950</v>
       </c>
@@ -12632,7 +12651,7 @@
       </c>
       <c r="H318" s="2"/>
     </row>
-    <row r="319" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>953</v>
       </c>
@@ -12656,7 +12675,7 @@
       </c>
       <c r="H319" s="2"/>
     </row>
-    <row r="320" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>956</v>
       </c>
@@ -12680,7 +12699,7 @@
       </c>
       <c r="H320" s="2"/>
     </row>
-    <row r="321" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>959</v>
       </c>
@@ -12704,7 +12723,7 @@
       </c>
       <c r="H321" s="2"/>
     </row>
-    <row r="322" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>961</v>
       </c>
@@ -12728,7 +12747,7 @@
       </c>
       <c r="H322" s="2"/>
     </row>
-    <row r="323" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>964</v>
       </c>
@@ -12752,7 +12771,7 @@
       </c>
       <c r="H323" s="2"/>
     </row>
-    <row r="324" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>967</v>
       </c>
@@ -12776,7 +12795,7 @@
       </c>
       <c r="H324" s="2"/>
     </row>
-    <row r="325" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>970</v>
       </c>
@@ -12800,7 +12819,7 @@
       </c>
       <c r="H325" s="2"/>
     </row>
-    <row r="326" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>973</v>
       </c>
@@ -12824,7 +12843,7 @@
         <v>1909</v>
       </c>
     </row>
-    <row r="327" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>975</v>
       </c>
@@ -12848,7 +12867,7 @@
         <v>1935</v>
       </c>
     </row>
-    <row r="328" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>977</v>
       </c>
@@ -12872,7 +12891,7 @@
       </c>
       <c r="H328" s="2"/>
     </row>
-    <row r="329" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>980</v>
       </c>
@@ -12896,7 +12915,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="330" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>984</v>
       </c>
@@ -12920,7 +12939,7 @@
       </c>
       <c r="H330" s="2"/>
     </row>
-    <row r="331" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>986</v>
       </c>
@@ -12944,7 +12963,7 @@
       </c>
       <c r="H331" s="2"/>
     </row>
-    <row r="332" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>989</v>
       </c>
@@ -12968,7 +12987,7 @@
       </c>
       <c r="H332" s="2"/>
     </row>
-    <row r="333" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>991</v>
       </c>
@@ -12992,7 +13011,7 @@
       </c>
       <c r="H333" s="2"/>
     </row>
-    <row r="334" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>993</v>
       </c>
@@ -13016,7 +13035,7 @@
       </c>
       <c r="H334" s="2"/>
     </row>
-    <row r="335" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>995</v>
       </c>
@@ -13040,7 +13059,7 @@
       </c>
       <c r="H335" s="2"/>
     </row>
-    <row r="336" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>997</v>
       </c>
@@ -13064,7 +13083,7 @@
       </c>
       <c r="H336" s="2"/>
     </row>
-    <row r="337" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>1000</v>
       </c>
@@ -13088,7 +13107,7 @@
       </c>
       <c r="H337" s="2"/>
     </row>
-    <row r="338" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>1004</v>
       </c>
@@ -13112,7 +13131,7 @@
       </c>
       <c r="H338" s="2"/>
     </row>
-    <row r="339" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>1006</v>
       </c>
@@ -13138,7 +13157,7 @@
         <v>1921</v>
       </c>
     </row>
-    <row r="340" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>1009</v>
       </c>
@@ -13162,7 +13181,7 @@
       </c>
       <c r="H340" s="2"/>
     </row>
-    <row r="341" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>1012</v>
       </c>
@@ -13186,7 +13205,7 @@
       </c>
       <c r="H341" s="2"/>
     </row>
-    <row r="342" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>1014</v>
       </c>
@@ -13210,7 +13229,7 @@
       </c>
       <c r="H342" s="2"/>
     </row>
-    <row r="343" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>1017</v>
       </c>
@@ -13234,7 +13253,7 @@
       </c>
       <c r="H343" s="2"/>
     </row>
-    <row r="344" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>1019</v>
       </c>
@@ -13258,7 +13277,7 @@
       </c>
       <c r="H344" s="2"/>
     </row>
-    <row r="345" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>1022</v>
       </c>
@@ -13282,7 +13301,7 @@
         <v>1912</v>
       </c>
     </row>
-    <row r="346" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>1025</v>
       </c>
@@ -13306,7 +13325,7 @@
       </c>
       <c r="H346" s="2"/>
     </row>
-    <row r="347" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>1027</v>
       </c>
@@ -13330,7 +13349,7 @@
       </c>
       <c r="H347" s="2"/>
     </row>
-    <row r="348" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>1029</v>
       </c>
@@ -13354,7 +13373,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="349" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>1033</v>
       </c>
@@ -13378,7 +13397,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="350" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>1035</v>
       </c>
@@ -13402,7 +13421,7 @@
       </c>
       <c r="H350" s="2"/>
     </row>
-    <row r="351" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>1038</v>
       </c>
@@ -13426,7 +13445,7 @@
       </c>
       <c r="H351" s="2"/>
     </row>
-    <row r="352" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>1040</v>
       </c>
@@ -13450,7 +13469,7 @@
       </c>
       <c r="H352" s="2"/>
     </row>
-    <row r="353" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>1043</v>
       </c>
@@ -13474,7 +13493,7 @@
       </c>
       <c r="H353" s="2"/>
     </row>
-    <row r="354" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>1046</v>
       </c>
@@ -13498,7 +13517,7 @@
       </c>
       <c r="H354" s="2"/>
     </row>
-    <row r="355" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>1048</v>
       </c>
@@ -13522,7 +13541,7 @@
       </c>
       <c r="H355" s="2"/>
     </row>
-    <row r="356" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>1051</v>
       </c>
@@ -13546,7 +13565,7 @@
       </c>
       <c r="H356" s="2"/>
     </row>
-    <row r="357" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>1053</v>
       </c>
@@ -13570,7 +13589,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="358" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>1055</v>
       </c>
@@ -13594,7 +13613,7 @@
       </c>
       <c r="H358" s="2"/>
     </row>
-    <row r="359" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>1058</v>
       </c>
@@ -13618,7 +13637,7 @@
       </c>
       <c r="H359" s="2"/>
     </row>
-    <row r="360" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>1061</v>
       </c>
@@ -13642,7 +13661,7 @@
       </c>
       <c r="H360" s="2"/>
     </row>
-    <row r="361" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>1063</v>
       </c>
@@ -13666,7 +13685,7 @@
       </c>
       <c r="H361" s="2"/>
     </row>
-    <row r="362" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>1065</v>
       </c>
@@ -13690,7 +13709,7 @@
       </c>
       <c r="H362" s="2"/>
     </row>
-    <row r="363" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>1067</v>
       </c>
@@ -13714,7 +13733,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="364" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>1070</v>
       </c>
@@ -13738,7 +13757,7 @@
       </c>
       <c r="H364" s="2"/>
     </row>
-    <row r="365" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>1072</v>
       </c>
@@ -13762,7 +13781,7 @@
       </c>
       <c r="H365" s="2"/>
     </row>
-    <row r="366" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>1075</v>
       </c>
@@ -13786,7 +13805,7 @@
       </c>
       <c r="H366" s="2"/>
     </row>
-    <row r="367" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>1079</v>
       </c>
@@ -13810,7 +13829,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="368" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>1082</v>
       </c>
@@ -13834,7 +13853,7 @@
       </c>
       <c r="H368" s="2"/>
     </row>
-    <row r="369" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>1085</v>
       </c>
@@ -13858,7 +13877,7 @@
       </c>
       <c r="H369" s="2"/>
     </row>
-    <row r="370" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>1087</v>
       </c>
@@ -13882,7 +13901,7 @@
         <v>1849</v>
       </c>
     </row>
-    <row r="371" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>1089</v>
       </c>
@@ -13906,7 +13925,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="372" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>1091</v>
       </c>
@@ -13930,7 +13949,7 @@
       </c>
       <c r="H372" s="2"/>
     </row>
-    <row r="373" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>1093</v>
       </c>
@@ -13954,7 +13973,7 @@
       </c>
       <c r="H373" s="2"/>
     </row>
-    <row r="374" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>1095</v>
       </c>
@@ -13978,7 +13997,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="375" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>1097</v>
       </c>
@@ -14002,7 +14021,7 @@
       </c>
       <c r="H375" s="2"/>
     </row>
-    <row r="376" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>1099</v>
       </c>
@@ -14026,7 +14045,7 @@
       </c>
       <c r="H376" s="2"/>
     </row>
-    <row r="377" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>1101</v>
       </c>
@@ -14050,7 +14069,7 @@
       </c>
       <c r="H377" s="2"/>
     </row>
-    <row r="378" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>1103</v>
       </c>
@@ -14074,7 +14093,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="379" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>1105</v>
       </c>
@@ -14096,7 +14115,7 @@
       </c>
       <c r="H379" s="2"/>
     </row>
-    <row r="380" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>1107</v>
       </c>
@@ -14120,7 +14139,7 @@
       </c>
       <c r="H380" s="2"/>
     </row>
-    <row r="381" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>1110</v>
       </c>
@@ -14144,7 +14163,7 @@
       </c>
       <c r="H381" s="2"/>
     </row>
-    <row r="382" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>1113</v>
       </c>
@@ -14168,7 +14187,7 @@
         <v>1837</v>
       </c>
     </row>
-    <row r="383" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>1115</v>
       </c>
@@ -14192,7 +14211,7 @@
       </c>
       <c r="H383" s="2"/>
     </row>
-    <row r="384" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>1118</v>
       </c>
@@ -14216,7 +14235,7 @@
       </c>
       <c r="H384" s="2"/>
     </row>
-    <row r="385" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>1120</v>
       </c>
@@ -14240,7 +14259,7 @@
       </c>
       <c r="H385" s="2"/>
     </row>
-    <row r="386" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>1123</v>
       </c>
@@ -14262,7 +14281,7 @@
       </c>
       <c r="H386" s="2"/>
     </row>
-    <row r="387" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>1125</v>
       </c>
@@ -14286,7 +14305,7 @@
       </c>
       <c r="H387" s="2"/>
     </row>
-    <row r="388" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>1127</v>
       </c>
@@ -14310,7 +14329,7 @@
       </c>
       <c r="H388" s="2"/>
     </row>
-    <row r="389" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>1129</v>
       </c>
@@ -14334,7 +14353,7 @@
       </c>
       <c r="H389" s="2"/>
     </row>
-    <row r="390" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>1131</v>
       </c>
@@ -14358,7 +14377,7 @@
       </c>
       <c r="H390" s="2"/>
     </row>
-    <row r="391" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>1134</v>
       </c>
@@ -14382,7 +14401,7 @@
       </c>
       <c r="H391" s="2"/>
     </row>
-    <row r="392" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>1136</v>
       </c>
@@ -14406,7 +14425,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="393" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>1138</v>
       </c>
@@ -14430,7 +14449,7 @@
       </c>
       <c r="H393" s="2"/>
     </row>
-    <row r="394" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>1141</v>
       </c>
@@ -14454,7 +14473,7 @@
       </c>
       <c r="H394" s="2"/>
     </row>
-    <row r="395" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>1144</v>
       </c>
@@ -14478,7 +14497,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="396" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>1146</v>
       </c>
@@ -14502,7 +14521,7 @@
       </c>
       <c r="H396" s="2"/>
     </row>
-    <row r="397" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>1148</v>
       </c>
@@ -14526,7 +14545,7 @@
       </c>
       <c r="H397" s="2"/>
     </row>
-    <row r="398" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>1150</v>
       </c>
@@ -14550,7 +14569,7 @@
       </c>
       <c r="H398" s="2"/>
     </row>
-    <row r="399" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>1152</v>
       </c>
@@ -14574,7 +14593,7 @@
       </c>
       <c r="H399" s="2"/>
     </row>
-    <row r="400" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>1155</v>
       </c>
@@ -14598,7 +14617,7 @@
       </c>
       <c r="H400" s="2"/>
     </row>
-    <row r="401" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>1158</v>
       </c>
@@ -14622,7 +14641,7 @@
       </c>
       <c r="H401" s="2"/>
     </row>
-    <row r="402" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>1161</v>
       </c>
@@ -14646,7 +14665,7 @@
       </c>
       <c r="H402" s="2"/>
     </row>
-    <row r="403" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>1163</v>
       </c>
@@ -14670,7 +14689,7 @@
       </c>
       <c r="H403" s="2"/>
     </row>
-    <row r="404" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>1166</v>
       </c>
@@ -14692,7 +14711,7 @@
       </c>
       <c r="H404" s="2"/>
     </row>
-    <row r="405" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>1168</v>
       </c>
@@ -14716,7 +14735,7 @@
       </c>
       <c r="H405" s="2"/>
     </row>
-    <row r="406" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>1171</v>
       </c>
@@ -14740,7 +14759,7 @@
       </c>
       <c r="H406" s="2"/>
     </row>
-    <row r="407" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>1174</v>
       </c>
@@ -14764,7 +14783,7 @@
       </c>
       <c r="H407" s="2"/>
     </row>
-    <row r="408" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>1176</v>
       </c>
@@ -14788,7 +14807,7 @@
       </c>
       <c r="H408" s="2"/>
     </row>
-    <row r="409" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>1178</v>
       </c>
@@ -14812,7 +14831,7 @@
       </c>
       <c r="H409" s="2"/>
     </row>
-    <row r="410" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>1180</v>
       </c>
@@ -14836,7 +14855,7 @@
       </c>
       <c r="H410" s="2"/>
     </row>
-    <row r="411" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>1183</v>
       </c>
@@ -14860,7 +14879,7 @@
       </c>
       <c r="H411" s="2"/>
     </row>
-    <row r="412" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>1186</v>
       </c>
@@ -14886,7 +14905,7 @@
         <v>1926</v>
       </c>
     </row>
-    <row r="413" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>1189</v>
       </c>
@@ -14910,7 +14929,7 @@
       </c>
       <c r="H413" s="2"/>
     </row>
-    <row r="414" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>1191</v>
       </c>
@@ -14932,7 +14951,7 @@
       </c>
       <c r="H414" s="2"/>
     </row>
-    <row r="415" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>1194</v>
       </c>
@@ -14954,7 +14973,7 @@
       </c>
       <c r="H415" s="2"/>
     </row>
-    <row r="416" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>1196</v>
       </c>
@@ -14980,7 +14999,7 @@
         <v>1866</v>
       </c>
     </row>
-    <row r="417" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>1198</v>
       </c>
@@ -15004,7 +15023,7 @@
       </c>
       <c r="H417" s="2"/>
     </row>
-    <row r="418" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>1200</v>
       </c>
@@ -15028,7 +15047,7 @@
       </c>
       <c r="H418" s="2"/>
     </row>
-    <row r="419" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>1203</v>
       </c>
@@ -15052,7 +15071,7 @@
       </c>
       <c r="H419" s="2"/>
     </row>
-    <row r="420" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>1205</v>
       </c>
@@ -15076,7 +15095,7 @@
       </c>
       <c r="H420" s="2"/>
     </row>
-    <row r="421" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>1209</v>
       </c>
@@ -15098,7 +15117,7 @@
       </c>
       <c r="H421" s="2"/>
     </row>
-    <row r="422" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>1211</v>
       </c>
@@ -15122,7 +15141,7 @@
       </c>
       <c r="H422" s="2"/>
     </row>
-    <row r="423" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>1213</v>
       </c>
@@ -15144,7 +15163,7 @@
       </c>
       <c r="H423" s="2"/>
     </row>
-    <row r="424" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>1215</v>
       </c>
@@ -15168,7 +15187,7 @@
       </c>
       <c r="H424" s="2"/>
     </row>
-    <row r="425" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>1218</v>
       </c>
@@ -15192,7 +15211,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="426" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>1220</v>
       </c>
@@ -15214,7 +15233,7 @@
       </c>
       <c r="H426" s="2"/>
     </row>
-    <row r="427" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>1222</v>
       </c>
@@ -15238,7 +15257,7 @@
       </c>
       <c r="H427" s="2"/>
     </row>
-    <row r="428" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>1224</v>
       </c>
@@ -15262,7 +15281,7 @@
       </c>
       <c r="H428" s="2"/>
     </row>
-    <row r="429" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>1227</v>
       </c>
@@ -15286,7 +15305,7 @@
       </c>
       <c r="H429" s="2"/>
     </row>
-    <row r="430" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>1229</v>
       </c>
@@ -15310,7 +15329,7 @@
       </c>
       <c r="H430" s="2"/>
     </row>
-    <row r="431" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>1231</v>
       </c>
@@ -15334,7 +15353,7 @@
       </c>
       <c r="H431" s="2"/>
     </row>
-    <row r="432" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>1233</v>
       </c>
@@ -15358,7 +15377,7 @@
       </c>
       <c r="H432" s="2"/>
     </row>
-    <row r="433" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>1235</v>
       </c>
@@ -15382,7 +15401,7 @@
       </c>
       <c r="H433" s="2"/>
     </row>
-    <row r="434" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>1237</v>
       </c>
@@ -15406,7 +15425,7 @@
       </c>
       <c r="H434" s="2"/>
     </row>
-    <row r="435" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>1240</v>
       </c>
@@ -15430,7 +15449,7 @@
         <v>1937</v>
       </c>
     </row>
-    <row r="436" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
         <v>1243</v>
       </c>
@@ -15454,7 +15473,7 @@
       </c>
       <c r="H436" s="2"/>
     </row>
-    <row r="437" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
         <v>1246</v>
       </c>
@@ -15478,7 +15497,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="438" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
         <v>1248</v>
       </c>
@@ -15502,7 +15521,7 @@
       </c>
       <c r="H438" s="2"/>
     </row>
-    <row r="439" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
         <v>1250</v>
       </c>
@@ -15526,7 +15545,7 @@
       </c>
       <c r="H439" s="2"/>
     </row>
-    <row r="440" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
         <v>1252</v>
       </c>
@@ -15550,7 +15569,7 @@
       </c>
       <c r="H440" s="2"/>
     </row>
-    <row r="441" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
         <v>1254</v>
       </c>
@@ -15574,7 +15593,7 @@
         <v>1930</v>
       </c>
     </row>
-    <row r="442" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
         <v>1256</v>
       </c>
@@ -15598,7 +15617,7 @@
       </c>
       <c r="H442" s="2"/>
     </row>
-    <row r="443" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
         <v>1258</v>
       </c>
@@ -15622,7 +15641,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="444" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
         <v>1260</v>
       </c>
@@ -15646,7 +15665,7 @@
       </c>
       <c r="H444" s="2"/>
     </row>
-    <row r="445" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
         <v>1262</v>
       </c>
@@ -15672,7 +15691,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="446" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
         <v>1264</v>
       </c>
@@ -15694,7 +15713,7 @@
       </c>
       <c r="H446" s="2"/>
     </row>
-    <row r="447" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
         <v>1266</v>
       </c>
@@ -15718,7 +15737,7 @@
       </c>
       <c r="H447" s="2"/>
     </row>
-    <row r="448" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
         <v>1269</v>
       </c>
@@ -15742,7 +15761,7 @@
       </c>
       <c r="H448" s="2"/>
     </row>
-    <row r="449" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
         <v>1272</v>
       </c>
@@ -15766,7 +15785,7 @@
       </c>
       <c r="H449" s="2"/>
     </row>
-    <row r="450" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
         <v>1274</v>
       </c>
@@ -15790,7 +15809,7 @@
       </c>
       <c r="H450" s="2"/>
     </row>
-    <row r="451" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
         <v>1277</v>
       </c>
@@ -15814,7 +15833,7 @@
       </c>
       <c r="H451" s="2"/>
     </row>
-    <row r="452" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
         <v>1279</v>
       </c>
@@ -15838,7 +15857,7 @@
       </c>
       <c r="H452" s="2"/>
     </row>
-    <row r="453" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
         <v>1281</v>
       </c>
@@ -15862,7 +15881,7 @@
       </c>
       <c r="H453" s="2"/>
     </row>
-    <row r="454" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
         <v>1284</v>
       </c>
@@ -15886,7 +15905,7 @@
       </c>
       <c r="H454" s="2"/>
     </row>
-    <row r="455" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
         <v>1286</v>
       </c>
@@ -15910,7 +15929,7 @@
       </c>
       <c r="H455" s="2"/>
     </row>
-    <row r="456" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
         <v>1288</v>
       </c>
@@ -15932,7 +15951,7 @@
       </c>
       <c r="H456" s="2"/>
     </row>
-    <row r="457" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
         <v>1291</v>
       </c>
@@ -15956,7 +15975,7 @@
       </c>
       <c r="H457" s="2"/>
     </row>
-    <row r="458" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
         <v>1294</v>
       </c>
@@ -15980,7 +15999,7 @@
       </c>
       <c r="H458" s="2"/>
     </row>
-    <row r="459" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
         <v>1297</v>
       </c>
@@ -16004,7 +16023,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="460" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
         <v>1299</v>
       </c>
@@ -16028,7 +16047,7 @@
       </c>
       <c r="H460" s="2"/>
     </row>
-    <row r="461" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
         <v>1301</v>
       </c>
@@ -16052,7 +16071,7 @@
       </c>
       <c r="H461" s="2"/>
     </row>
-    <row r="462" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
         <v>1303</v>
       </c>
@@ -16074,7 +16093,7 @@
       </c>
       <c r="H462" s="2"/>
     </row>
-    <row r="463" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
         <v>1305</v>
       </c>
@@ -16098,7 +16117,7 @@
       </c>
       <c r="H463" s="2"/>
     </row>
-    <row r="464" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
         <v>1307</v>
       </c>
@@ -16122,7 +16141,7 @@
       </c>
       <c r="H464" s="2"/>
     </row>
-    <row r="465" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
         <v>1310</v>
       </c>
@@ -16146,7 +16165,7 @@
       </c>
       <c r="H465" s="2"/>
     </row>
-    <row r="466" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
         <v>1312</v>
       </c>
@@ -16170,7 +16189,7 @@
       </c>
       <c r="H466" s="2"/>
     </row>
-    <row r="467" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
         <v>1315</v>
       </c>
@@ -16192,7 +16211,7 @@
       </c>
       <c r="H467" s="2"/>
     </row>
-    <row r="468" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
         <v>1317</v>
       </c>
@@ -16216,7 +16235,7 @@
       </c>
       <c r="H468" s="2"/>
     </row>
-    <row r="469" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
         <v>1320</v>
       </c>
@@ -16240,7 +16259,7 @@
       </c>
       <c r="H469" s="2"/>
     </row>
-    <row r="470" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
         <v>1323</v>
       </c>
@@ -16264,7 +16283,7 @@
       </c>
       <c r="H470" s="2"/>
     </row>
-    <row r="471" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
         <v>1325</v>
       </c>
@@ -16288,7 +16307,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="472" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
         <v>1327</v>
       </c>
@@ -16312,7 +16331,7 @@
       </c>
       <c r="H472" s="2"/>
     </row>
-    <row r="473" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
         <v>1329</v>
       </c>
@@ -16336,7 +16355,7 @@
       </c>
       <c r="H473" s="2"/>
     </row>
-    <row r="474" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
         <v>1331</v>
       </c>
@@ -16360,7 +16379,7 @@
       </c>
       <c r="H474" s="2"/>
     </row>
-    <row r="475" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
         <v>1334</v>
       </c>
@@ -16384,7 +16403,7 @@
       </c>
       <c r="H475" s="2"/>
     </row>
-    <row r="476" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
         <v>1337</v>
       </c>
@@ -16408,7 +16427,7 @@
       </c>
       <c r="H476" s="2"/>
     </row>
-    <row r="477" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
         <v>1339</v>
       </c>
@@ -16432,7 +16451,7 @@
       </c>
       <c r="H477" s="2"/>
     </row>
-    <row r="478" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
         <v>1341</v>
       </c>
@@ -16454,7 +16473,7 @@
       </c>
       <c r="H478" s="2"/>
     </row>
-    <row r="479" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
         <v>1343</v>
       </c>
@@ -16478,7 +16497,7 @@
       </c>
       <c r="H479" s="2"/>
     </row>
-    <row r="480" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
         <v>1345</v>
       </c>
@@ -16500,7 +16519,7 @@
       </c>
       <c r="H480" s="2"/>
     </row>
-    <row r="481" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
         <v>1347</v>
       </c>
@@ -16524,7 +16543,7 @@
       </c>
       <c r="H481" s="2"/>
     </row>
-    <row r="482" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
         <v>1349</v>
       </c>
@@ -16548,7 +16567,7 @@
       </c>
       <c r="H482" s="2"/>
     </row>
-    <row r="483" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
         <v>1352</v>
       </c>
@@ -16572,7 +16591,7 @@
       </c>
       <c r="H483" s="2"/>
     </row>
-    <row r="484" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
         <v>1354</v>
       </c>
@@ -16596,7 +16615,7 @@
       </c>
       <c r="H484" s="2"/>
     </row>
-    <row r="485" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A485" t="s">
         <v>1357</v>
       </c>
@@ -16620,7 +16639,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="486" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
         <v>1359</v>
       </c>
@@ -16644,7 +16663,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="487" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A487" t="s">
         <v>1362</v>
       </c>
@@ -16668,7 +16687,7 @@
       </c>
       <c r="H487" s="2"/>
     </row>
-    <row r="488" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
         <v>1364</v>
       </c>
@@ -16692,7 +16711,7 @@
       </c>
       <c r="H488" s="2"/>
     </row>
-    <row r="489" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
         <v>1366</v>
       </c>
@@ -16716,7 +16735,7 @@
       </c>
       <c r="H489" s="2"/>
     </row>
-    <row r="490" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A490" t="s">
         <v>1369</v>
       </c>
@@ -16740,7 +16759,7 @@
       </c>
       <c r="H490" s="2"/>
     </row>
-    <row r="491" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
         <v>1371</v>
       </c>
@@ -16764,7 +16783,7 @@
         <v>1851</v>
       </c>
     </row>
-    <row r="492" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A492" t="s">
         <v>1374</v>
       </c>
@@ -16786,7 +16805,7 @@
       </c>
       <c r="H492" s="2"/>
     </row>
-    <row r="493" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
         <v>1376</v>
       </c>
@@ -16808,7 +16827,7 @@
       </c>
       <c r="H493" s="2"/>
     </row>
-    <row r="494" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
         <v>1379</v>
       </c>
@@ -16832,7 +16851,7 @@
         <v>1911</v>
       </c>
     </row>
-    <row r="495" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
         <v>1382</v>
       </c>
@@ -16856,7 +16875,7 @@
       </c>
       <c r="H495" s="2"/>
     </row>
-    <row r="496" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
         <v>1384</v>
       </c>
@@ -16880,7 +16899,7 @@
       </c>
       <c r="H496" s="2"/>
     </row>
-    <row r="497" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A497" t="s">
         <v>1387</v>
       </c>
@@ -16904,7 +16923,7 @@
       </c>
       <c r="H497" s="2"/>
     </row>
-    <row r="498" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A498" t="s">
         <v>1389</v>
       </c>
@@ -16928,7 +16947,7 @@
         <v>1909</v>
       </c>
     </row>
-    <row r="499" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A499" t="s">
         <v>1391</v>
       </c>
@@ -16952,7 +16971,7 @@
         <v>1906</v>
       </c>
     </row>
-    <row r="500" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A500" t="s">
         <v>1393</v>
       </c>
@@ -16976,7 +16995,7 @@
       </c>
       <c r="H500" s="2"/>
     </row>
-    <row r="501" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
         <v>1395</v>
       </c>
@@ -17000,7 +17019,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="502" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A502" t="s">
         <v>1397</v>
       </c>
@@ -17024,7 +17043,7 @@
       </c>
       <c r="H502" s="2"/>
     </row>
-    <row r="503" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A503" t="s">
         <v>1400</v>
       </c>
@@ -17048,7 +17067,7 @@
       </c>
       <c r="H503" s="2"/>
     </row>
-    <row r="504" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A504" t="s">
         <v>1402</v>
       </c>
@@ -17072,7 +17091,7 @@
       </c>
       <c r="H504" s="2"/>
     </row>
-    <row r="505" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A505" t="s">
         <v>1405</v>
       </c>
@@ -17096,7 +17115,7 @@
       </c>
       <c r="H505" s="2"/>
     </row>
-    <row r="506" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A506" t="s">
         <v>1407</v>
       </c>
@@ -17120,6 +17139,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H506"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>